<commit_message>
rework for error check round 1
</commit_message>
<xml_diff>
--- a/กราฟการทำงานของ ABB.xlsx
+++ b/กราฟการทำงานของ ABB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\icanfly37\Documents\GitHub\excel-graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754848F4-5E73-43D1-9814-6CF1E8229C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB72E4F0-1156-4D6D-A8F3-8D77DFBBA571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="35610" windowHeight="13320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="35610" windowHeight="13320" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ABB1" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="ABB4" sheetId="3" r:id="rId3"/>
     <sheet name="ตัวอย่างกราฟ" sheetId="4" r:id="rId4"/>
     <sheet name="Graph Timing ABB1" sheetId="5" r:id="rId5"/>
+    <sheet name="TestError" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1536" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="176">
   <si>
     <t>ชื่อสินค้า</t>
   </si>
@@ -534,6 +535,24 @@
   </si>
   <si>
     <t>T-2311&lt;--GEAR OIL EP 460</t>
+  </si>
+  <si>
+    <t>AAA</t>
+  </si>
+  <si>
+    <t>BBB</t>
+  </si>
+  <si>
+    <t>03/05/2567</t>
+  </si>
+  <si>
+    <t>CCC</t>
+  </si>
+  <si>
+    <t>04/05/2568</t>
+  </si>
+  <si>
+    <t>15:37</t>
   </si>
 </sst>
 </file>
@@ -1034,8 +1053,8 @@
   <dimension ref="A1:E177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.5" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4064,7 +4083,7 @@
   <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5639,7 +5658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AX52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
@@ -6725,4 +6744,93 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.125" style="17" customWidth="1"/>
+    <col min="2" max="3" width="18" style="17" customWidth="1"/>
+    <col min="4" max="4" width="18.125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="18" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>